<commit_message>
day2 - API and write into excel
</commit_message>
<xml_diff>
--- a/Day1-Excel-MultiSheet dan Append/fileAppend.xlsx
+++ b/Day1-Excel-MultiSheet dan Append/fileAppend.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>No</t>
   </si>
@@ -52,25 +52,10 @@
     <t>Jakarta</t>
   </si>
   <si>
-    <t>Nadia Ningtias</t>
-  </si>
-  <si>
-    <t>Sidoarjo</t>
-  </si>
-  <si>
-    <t>Rahmad ksmrdn</t>
-  </si>
-  <si>
-    <t>Novita</t>
-  </si>
-  <si>
-    <t>Denpasar</t>
-  </si>
-  <si>
-    <t>Linda</t>
-  </si>
-  <si>
-    <t>Solo</t>
+    <t>Nadia</t>
+  </si>
+  <si>
+    <t>surabaya</t>
   </si>
 </sst>
 </file>
@@ -402,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -463,39 +448,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>